<commit_message>
bug fix for reader
</commit_message>
<xml_diff>
--- a/RoperALZDataMigration/RoperSpreadSheet2.xlsx
+++ b/RoperALZDataMigration/RoperSpreadSheet2.xlsx
@@ -1,46 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\git\rsfh-alz-intake-b\java\RoperALZIntake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF84158-A1B1-4955-B5F4-D4B5FF2F9F5A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{5EF84158-A1B1-4955-B5F4-D4B5FF2F9F5A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7848" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="1" windowHeight="7848" windowWidth="17256" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Participant Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Symptoms" sheetId="7" r:id="rId2"/>
-    <sheet name="HPOA" sheetId="8" r:id="rId3"/>
-    <sheet name="Medical History" sheetId="9" r:id="rId4"/>
-    <sheet name="Status" sheetId="11" r:id="rId5"/>
-    <sheet name="Test Scores" sheetId="4" r:id="rId6"/>
-    <sheet name="Referral Sheet" sheetId="2" r:id="rId7"/>
-    <sheet name="Current Studies" sheetId="6" r:id="rId8"/>
-    <sheet name="OptInEamils" sheetId="3" r:id="rId9"/>
-    <sheet name="Formulas&amp;Tables" sheetId="5" r:id="rId10"/>
+    <sheet name="Participant Data" r:id="rId1" sheetId="1"/>
+    <sheet name="Symptoms" r:id="rId2" sheetId="7"/>
+    <sheet name="HPOA" r:id="rId3" sheetId="8"/>
+    <sheet name="Medical History" r:id="rId4" sheetId="9"/>
+    <sheet name="Status" r:id="rId5" sheetId="11"/>
+    <sheet name="Test Scores" r:id="rId6" sheetId="4"/>
+    <sheet name="Referral Sheet" r:id="rId7" sheetId="2"/>
+    <sheet name="Current Studies" r:id="rId8" sheetId="6"/>
+    <sheet name="OptInEamils" r:id="rId9" sheetId="3"/>
+    <sheet name="Formulas&amp;Tables" r:id="rId10" sheetId="5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_newdatabase.xlsxTable11" hidden="1">Referals[]</definedName>
+    <definedName hidden="1" name="_xlcn.WorksheetConnection_newdatabase.xlsxTable11">Referals[]</definedName>
     <definedName name="termReason">'Formulas&amp;Tables'!$B$3:$B$6</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
+    <ext uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
       <x15:dataModel>
         <x15:modelTables>
-          <x15:modelTable id="Table2" name="Table2" connection="WorksheetConnection_new database.xlsx!Table2"/>
-          <x15:modelTable id="Table1" name="Table1" connection="WorksheetConnection_new database.xlsx!Table1"/>
+          <x15:modelTable connection="WorksheetConnection_new database.xlsx!Table2" id="Table2" name="Table2"/>
+          <x15:modelTable connection="WorksheetConnection_new database.xlsx!Table1" id="Table1" name="Table1"/>
         </x15:modelTables>
         <x15:modelRelationships>
-          <x15:modelRelationship fromTable="Table1" fromColumn="Column1" toTable="Table2" toColumn="Column1"/>
+          <x15:modelRelationship fromColumn="Column1" fromTable="Table1" toColumn="Column1" toTable="Table2"/>
         </x15:modelRelationships>
       </x15:dataModel>
     </ext>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="217">
   <si>
     <t>Last Name</t>
   </si>
@@ -531,15 +531,208 @@
   </si>
   <si>
     <t>Dementia (unspecified)</t>
+  </si>
+  <si>
+    <t>WELLS</t>
+  </si>
+  <si>
+    <t>PATRICK</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>545 ABBEY ST</t>
+  </si>
+  <si>
+    <t>Charleston</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>29401</t>
+  </si>
+  <si>
+    <t>patrick.wells@uf.edu</t>
+  </si>
+  <si>
+    <t>CROSS</t>
+  </si>
+  <si>
+    <t>DARREN</t>
+  </si>
+  <si>
+    <t>926 ABBEY ST</t>
+  </si>
+  <si>
+    <t>darren.cross@trident.edu</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>CHURCH</t>
+  </si>
+  <si>
+    <t>JENNIE</t>
+  </si>
+  <si>
+    <t>101 ACACIA AVE</t>
+  </si>
+  <si>
+    <t>jennie.church@mail.com</t>
+  </si>
+  <si>
+    <t>William Snyder</t>
+  </si>
+  <si>
+    <t>WANG</t>
+  </si>
+  <si>
+    <t>AMY</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>532 ACACIA AVE</t>
+  </si>
+  <si>
+    <t>amy.wang@yahoo.com</t>
+  </si>
+  <si>
+    <t>Dr. Curtis Haskins</t>
+  </si>
+  <si>
+    <t>JENSEN</t>
+  </si>
+  <si>
+    <t>JANICE</t>
+  </si>
+  <si>
+    <t>149 ACACIA ST</t>
+  </si>
+  <si>
+    <t>janice.jensen@yahoo.com</t>
+  </si>
+  <si>
+    <t>Egleston</t>
+  </si>
+  <si>
+    <t>30/27</t>
+  </si>
+  <si>
+    <t>ACEVEDO</t>
+  </si>
+  <si>
+    <t>FELICIA</t>
+  </si>
+  <si>
+    <t>16 ACACIA ST</t>
+  </si>
+  <si>
+    <t>felicia.acevedo@usa.gov</t>
+  </si>
+  <si>
+    <t>Palmetto Primary Care</t>
+  </si>
+  <si>
+    <t>DOYLE</t>
+  </si>
+  <si>
+    <t>JAY</t>
+  </si>
+  <si>
+    <t>515 ACADIA ST</t>
+  </si>
+  <si>
+    <t>jay.doyle@yahoo.com</t>
+  </si>
+  <si>
+    <t>WHITEHEAD</t>
+  </si>
+  <si>
+    <t>BETTY</t>
+  </si>
+  <si>
+    <t>465 ACADIA ST</t>
+  </si>
+  <si>
+    <t>betty.whitehead@att.net</t>
+  </si>
+  <si>
+    <t>Dr. K. Bolus</t>
+  </si>
+  <si>
+    <t>27/27</t>
+  </si>
+  <si>
+    <t>MCCLURE</t>
+  </si>
+  <si>
+    <t>STACEY</t>
+  </si>
+  <si>
+    <t>972 ACEVEDO AVE</t>
+  </si>
+  <si>
+    <t>stacey.mcclure@gamil.com</t>
+  </si>
+  <si>
+    <t>LINDSAY</t>
+  </si>
+  <si>
+    <t>PRISCILLA</t>
+  </si>
+  <si>
+    <t>777 ACEVEDO AVE</t>
+  </si>
+  <si>
+    <t>priscilla.lindsay@comcast.net</t>
+  </si>
+  <si>
+    <t>ORTEGA</t>
+  </si>
+  <si>
+    <t>VINCENT</t>
+  </si>
+  <si>
+    <t>974 ACME ALY</t>
+  </si>
+  <si>
+    <t>vincent.ortega@mail.com</t>
+  </si>
+  <si>
+    <t>632-677-1278</t>
+  </si>
+  <si>
+    <t>30/30</t>
+  </si>
+  <si>
+    <t>BEACH</t>
+  </si>
+  <si>
+    <t>MABEL</t>
+  </si>
+  <si>
+    <t>454 ACME ALY</t>
+  </si>
+  <si>
+    <t>mabel.beach@aol.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="166" formatCode="MM/dd/yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -633,115 +826,162 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="69">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="3" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="21">
     <dxf>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+      <numFmt formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####" numFmtId="164"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+      <numFmt formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####" numFmtId="164"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt formatCode="General" numFmtId="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+      <numFmt formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####" numFmtId="164"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+      <numFmt formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####" numFmtId="164"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt formatCode="0" numFmtId="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt formatCode="m/d/yyyy" numFmtId="19"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -754,102 +994,102 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Main" displayName="Main" ref="B3:X4" insertRow="1" insertRowShift="1" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" displayName="Main" id="3" insertRow="1" insertRowShift="1" mc:Ignorable="xr xr3" name="Main" ref="B3:X4" totalsRowShown="0" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}">
   <autoFilter ref="B3:X4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Last Name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="First Name"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DOB" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="age" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Race"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Gender"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Address"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Address 2"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="City"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="State"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Postal Code"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Email Address"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Phone Number" dataDxfId="18"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Test Date" dataDxfId="17"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="W - Score" dataDxfId="16"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="7s - Score" dataDxfId="15"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Status" dataDxfId="14"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Deseased" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="PCP"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Specialist"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Current Study"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Referral"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Mailing List"/>
+    <tableColumn id="1" name="Last Name" xr3:uid="{00000000-0010-0000-0000-000001000000}"/>
+    <tableColumn id="2" name="First Name" xr3:uid="{00000000-0010-0000-0000-000002000000}"/>
+    <tableColumn dataDxfId="20" id="3" name="DOB" xr3:uid="{00000000-0010-0000-0000-000003000000}"/>
+    <tableColumn dataDxfId="19" id="4" name="age" xr3:uid="{00000000-0010-0000-0000-000004000000}"/>
+    <tableColumn id="5" name="Race" xr3:uid="{00000000-0010-0000-0000-000005000000}"/>
+    <tableColumn id="6" name="Gender" xr3:uid="{00000000-0010-0000-0000-000006000000}"/>
+    <tableColumn id="7" name="Address" xr3:uid="{00000000-0010-0000-0000-000007000000}"/>
+    <tableColumn id="20" name="Address 2" xr3:uid="{00000000-0010-0000-0000-000014000000}"/>
+    <tableColumn id="21" name="City" xr3:uid="{00000000-0010-0000-0000-000015000000}"/>
+    <tableColumn id="19" name="State" xr3:uid="{00000000-0010-0000-0000-000013000000}"/>
+    <tableColumn id="22" name="Postal Code" xr3:uid="{00000000-0010-0000-0000-000016000000}"/>
+    <tableColumn id="8" name="Email Address" xr3:uid="{00000000-0010-0000-0000-000008000000}"/>
+    <tableColumn dataDxfId="18" id="9" name="Phone Number" xr3:uid="{00000000-0010-0000-0000-000009000000}"/>
+    <tableColumn dataDxfId="17" id="15" name="Test Date" xr3:uid="{00000000-0010-0000-0000-00000F000000}"/>
+    <tableColumn dataDxfId="16" id="16" name="W - Score" xr3:uid="{00000000-0010-0000-0000-000010000000}"/>
+    <tableColumn dataDxfId="15" id="17" name="7s - Score" xr3:uid="{00000000-0010-0000-0000-000011000000}"/>
+    <tableColumn dataDxfId="14" id="14" name="Status" xr3:uid="{00000000-0010-0000-0000-00000E000000}"/>
+    <tableColumn dataDxfId="13" id="23" name="Deseased" xr3:uid="{00000000-0010-0000-0000-000017000000}"/>
+    <tableColumn id="10" name="PCP" xr3:uid="{00000000-0010-0000-0000-00000A000000}"/>
+    <tableColumn id="11" name="Specialist" xr3:uid="{00000000-0010-0000-0000-00000B000000}"/>
+    <tableColumn id="25" name="Current Study" xr3:uid="{00000000-0010-0000-0000-000019000000}"/>
+    <tableColumn id="12" name="Referral" xr3:uid="{00000000-0010-0000-0000-00000C000000}"/>
+    <tableColumn id="13" name="Mailing List" xr3:uid="{00000000-0010-0000-0000-00000D000000}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table8" displayName="Table8" ref="B1:L2" insertRow="1" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" dataDxfId="11" displayName="Table8" headerRowDxfId="12" id="8" insertRow="1" mc:Ignorable="xr xr3" name="Table8" ref="B1:L2" totalsRowShown="0" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}">
   <autoFilter ref="B1:L2" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="First Name" dataDxfId="10"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="Last Name" dataDxfId="9"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="HOPA (yes/no)" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Phone" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Legally Married" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Spouse" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Phone2" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Children" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Names" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Phones" dataDxfId="0"/>
+    <tableColumn dataDxfId="10" id="1" name="First Name" xr3:uid="{00000000-0010-0000-0100-000001000000}"/>
+    <tableColumn dataDxfId="9" id="22" name="Last Name" xr3:uid="{00000000-0010-0000-0100-000016000000}"/>
+    <tableColumn dataDxfId="8" id="21" name="HOPA (yes/no)" xr3:uid="{00000000-0010-0000-0100-000015000000}"/>
+    <tableColumn dataDxfId="7" id="2" name="Name" xr3:uid="{00000000-0010-0000-0100-000002000000}"/>
+    <tableColumn dataDxfId="6" id="3" name="Phone" xr3:uid="{00000000-0010-0000-0100-000003000000}"/>
+    <tableColumn dataDxfId="5" id="4" name="Legally Married" xr3:uid="{00000000-0010-0000-0100-000004000000}"/>
+    <tableColumn dataDxfId="4" id="5" name="Spouse" xr3:uid="{00000000-0010-0000-0100-000005000000}"/>
+    <tableColumn dataDxfId="3" id="6" name="Phone2" xr3:uid="{00000000-0010-0000-0100-000006000000}"/>
+    <tableColumn dataDxfId="2" id="7" name="Children" xr3:uid="{00000000-0010-0000-0100-000007000000}"/>
+    <tableColumn dataDxfId="1" id="8" name="Names" xr3:uid="{00000000-0010-0000-0100-000008000000}"/>
+    <tableColumn dataDxfId="0" id="9" name="Phones" xr3:uid="{00000000-0010-0000-0100-000009000000}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table9" displayName="Table9" ref="B1:J2" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" displayName="Table9" id="9" mc:Ignorable="xr xr3" name="Table9" ref="B1:J2" totalsRowShown="0" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}">
   <autoFilter ref="B1:J2" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="First Name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Last Name"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Schizophrenia,Bipolar, Major Depressive Disorder"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Sleep Disorder"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Cancer"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Type of cancer"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Pacemaker or MRI incompatible Device"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Drug or alchohol abuse"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="On Going Problems"/>
+    <tableColumn id="1" name="First Name" xr3:uid="{00000000-0010-0000-0200-000001000000}"/>
+    <tableColumn id="2" name="Last Name" xr3:uid="{00000000-0010-0000-0200-000002000000}"/>
+    <tableColumn id="3" name="Schizophrenia,Bipolar, Major Depressive Disorder" xr3:uid="{00000000-0010-0000-0200-000003000000}"/>
+    <tableColumn id="4" name="Sleep Disorder" xr3:uid="{00000000-0010-0000-0200-000004000000}"/>
+    <tableColumn id="5" name="Cancer" xr3:uid="{00000000-0010-0000-0200-000005000000}"/>
+    <tableColumn id="6" name="Type of cancer" xr3:uid="{00000000-0010-0000-0200-000006000000}"/>
+    <tableColumn id="7" name="Pacemaker or MRI incompatible Device" xr3:uid="{00000000-0010-0000-0200-000007000000}"/>
+    <tableColumn id="8" name="Drug or alchohol abuse" xr3:uid="{00000000-0010-0000-0200-000008000000}"/>
+    <tableColumn id="9" name="On Going Problems" xr3:uid="{00000000-0010-0000-0200-000009000000}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Referals" displayName="Referals" ref="B2:B30" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" displayName="Referals" id="1" mc:Ignorable="xr xr3" name="Referals" ref="B2:B30" totalsRowShown="0" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}">
   <autoFilter ref="B2:B30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Referals"/>
+    <tableColumn id="1" name="Referals" xr3:uid="{00000000-0010-0000-0400-000001000000}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Studies" displayName="Studies" ref="B2:B11" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" displayName="Studies" id="7" mc:Ignorable="xr xr3" name="Studies" ref="B2:B11" totalsRowShown="0" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}">
   <autoFilter ref="B2:B11" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Studies"/>
+    <tableColumn id="1" name="Studies" xr3:uid="{00000000-0010-0000-0500-000001000000}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Emails" displayName="Emails" ref="B2:B32" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" displayName="Emails" id="6" mc:Ignorable="xr xr3" name="Emails" ref="B2:B32" totalsRowShown="0" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}">
   <autoFilter ref="B2:B32" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="OptInEmails"/>
+    <tableColumn id="1" name="OptInEmails" xr3:uid="{00000000-0010-0000-0600-000001000000}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
@@ -858,10 +1098,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -896,7 +1136,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -931,7 +1171,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1025,21 +1265,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1056,7 +1296,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1108,16 +1348,16 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:AW10"/>
+  <dimension ref="B1:Y57"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
@@ -1125,28 +1365,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.6640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="12" width="21.109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="25.109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.5546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.5546875" style="2" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="1.5546875" style="2" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="2.44140625" style="2" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="31" style="2" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="12.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="24" customWidth="1" collapsed="1"/>
-    <col min="21" max="22" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="15.88671875" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="20.44140625" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="28.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="10.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="9.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="8" max="12" customWidth="true" width="21.109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="25.109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="2" width="16.5546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" hidden="true" style="2" width="16.5546875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" hidden="true" style="2" width="1.5546875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" hidden="true" style="2" width="2.44140625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="2" width="31.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="2" width="12.44140625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="21" max="22" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="28.44140625" collapsed="true"/>
+    <col min="49" max="49" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row customHeight="1" ht="15" r="1" spans="2:24" x14ac:dyDescent="0.7">
       <c r="B1" s="4" t="s">
         <v>46</v>
       </c>
@@ -1285,7 +1525,7 @@
         <v>25359</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E10" ca="1" si="0">IF(ISBLANK(D5), "", (DATEDIF(D5, NOW(), "Y")))</f>
+        <f ca="1" ref="E5:E10" si="0" t="shared">IF(ISBLANK(D5), "", (DATEDIF(D5, NOW(), "Y")))</f>
         <v>49</v>
       </c>
       <c r="F5" t="s">
@@ -1342,7 +1582,7 @@
         <v>25359</v>
       </c>
       <c r="E6">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1" si="0" t="shared"/>
         <v>49</v>
       </c>
       <c r="F6" t="s">
@@ -1399,7 +1639,7 @@
         <v>25359</v>
       </c>
       <c r="E7">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1" si="0" t="shared"/>
         <v>49</v>
       </c>
       <c r="F7" t="s">
@@ -1456,7 +1696,7 @@
         <v>25359</v>
       </c>
       <c r="E8">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1" si="0" t="shared"/>
         <v>49</v>
       </c>
       <c r="F8" t="s">
@@ -1513,7 +1753,7 @@
         <v>25329</v>
       </c>
       <c r="E9">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1" si="0" t="shared"/>
         <v>49</v>
       </c>
       <c r="F9" t="s">
@@ -1570,7 +1810,7 @@
         <v>25329</v>
       </c>
       <c r="E10">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1" si="0" t="shared"/>
         <v>49</v>
       </c>
       <c r="F10" t="s">
@@ -1616,9 +1856,2085 @@
         <v>137</v>
       </c>
     </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11" s="22" t="n">
+        <v>14198.0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I11" t="s">
+        <v>158</v>
+      </c>
+      <c r="J11" t="s">
+        <v>159</v>
+      </c>
+      <c r="K11" t="s">
+        <v>160</v>
+      </c>
+      <c r="L11" t="s">
+        <v>161</v>
+      </c>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="P11" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>134</v>
+      </c>
+      <c r="R11" t="s">
+        <v>134</v>
+      </c>
+      <c r="S11"/>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D12" s="23" t="n">
+        <v>15962.0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>134</v>
+      </c>
+      <c r="G12" t="s">
+        <v>156</v>
+      </c>
+      <c r="H12" t="s">
+        <v>164</v>
+      </c>
+      <c r="I12" t="s">
+        <v>158</v>
+      </c>
+      <c r="J12" t="s">
+        <v>159</v>
+      </c>
+      <c r="K12" t="s">
+        <v>160</v>
+      </c>
+      <c r="L12" t="s">
+        <v>165</v>
+      </c>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="P12" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>134</v>
+      </c>
+      <c r="R12" t="s">
+        <v>166</v>
+      </c>
+      <c r="S12"/>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="24" t="n">
+        <v>13466.0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>155</v>
+      </c>
+      <c r="G13" t="s">
+        <v>156</v>
+      </c>
+      <c r="H13" t="s">
+        <v>169</v>
+      </c>
+      <c r="I13" t="s">
+        <v>158</v>
+      </c>
+      <c r="J13" t="s">
+        <v>159</v>
+      </c>
+      <c r="K13" t="s">
+        <v>160</v>
+      </c>
+      <c r="L13" t="s">
+        <v>170</v>
+      </c>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="P13" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>134</v>
+      </c>
+      <c r="R13" t="s">
+        <v>134</v>
+      </c>
+      <c r="S13"/>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" t="s">
+        <v>173</v>
+      </c>
+      <c r="D14" s="25" t="n">
+        <v>23463.0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>134</v>
+      </c>
+      <c r="G14" t="s">
+        <v>174</v>
+      </c>
+      <c r="H14" t="s">
+        <v>175</v>
+      </c>
+      <c r="I14" t="s">
+        <v>158</v>
+      </c>
+      <c r="J14" t="s">
+        <v>159</v>
+      </c>
+      <c r="K14" t="s">
+        <v>160</v>
+      </c>
+      <c r="L14" t="s">
+        <v>176</v>
+      </c>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="P14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>134</v>
+      </c>
+      <c r="R14" t="s">
+        <v>166</v>
+      </c>
+      <c r="S14"/>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>178</v>
+      </c>
+      <c r="C15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D15" s="26" t="n">
+        <v>11085.0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>134</v>
+      </c>
+      <c r="G15" t="s">
+        <v>156</v>
+      </c>
+      <c r="H15" t="s">
+        <v>180</v>
+      </c>
+      <c r="I15" t="s">
+        <v>158</v>
+      </c>
+      <c r="J15" t="s">
+        <v>159</v>
+      </c>
+      <c r="K15" t="s">
+        <v>160</v>
+      </c>
+      <c r="L15" t="s">
+        <v>181</v>
+      </c>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="P15" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>134</v>
+      </c>
+      <c r="R15" t="s">
+        <v>134</v>
+      </c>
+      <c r="S15"/>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>184</v>
+      </c>
+      <c r="C16" t="s">
+        <v>185</v>
+      </c>
+      <c r="D16" s="27" t="n">
+        <v>21738.0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>134</v>
+      </c>
+      <c r="G16" t="s">
+        <v>156</v>
+      </c>
+      <c r="H16" t="s">
+        <v>186</v>
+      </c>
+      <c r="I16" t="s">
+        <v>158</v>
+      </c>
+      <c r="J16" t="s">
+        <v>159</v>
+      </c>
+      <c r="K16" t="s">
+        <v>160</v>
+      </c>
+      <c r="L16" t="s">
+        <v>187</v>
+      </c>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="P16" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>134</v>
+      </c>
+      <c r="R16" t="s">
+        <v>166</v>
+      </c>
+      <c r="S16"/>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D17" s="28" t="n">
+        <v>9319.0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>134</v>
+      </c>
+      <c r="G17" t="s">
+        <v>156</v>
+      </c>
+      <c r="H17" t="s">
+        <v>191</v>
+      </c>
+      <c r="I17" t="s">
+        <v>158</v>
+      </c>
+      <c r="J17" t="s">
+        <v>159</v>
+      </c>
+      <c r="K17" t="s">
+        <v>160</v>
+      </c>
+      <c r="L17" t="s">
+        <v>192</v>
+      </c>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="P17" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>134</v>
+      </c>
+      <c r="R17" t="s">
+        <v>134</v>
+      </c>
+      <c r="S17"/>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>193</v>
+      </c>
+      <c r="C18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D18" s="29" t="n">
+        <v>21385.0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>134</v>
+      </c>
+      <c r="G18" t="s">
+        <v>156</v>
+      </c>
+      <c r="H18" t="s">
+        <v>195</v>
+      </c>
+      <c r="I18" t="s">
+        <v>158</v>
+      </c>
+      <c r="J18" t="s">
+        <v>159</v>
+      </c>
+      <c r="K18" t="s">
+        <v>160</v>
+      </c>
+      <c r="L18" t="s">
+        <v>196</v>
+      </c>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="P18" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>134</v>
+      </c>
+      <c r="R18" t="s">
+        <v>166</v>
+      </c>
+      <c r="S18"/>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>199</v>
+      </c>
+      <c r="C19" t="s">
+        <v>200</v>
+      </c>
+      <c r="D19" s="30" t="n">
+        <v>10690.0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G19" t="s">
+        <v>174</v>
+      </c>
+      <c r="H19" t="s">
+        <v>201</v>
+      </c>
+      <c r="I19" t="s">
+        <v>158</v>
+      </c>
+      <c r="J19" t="s">
+        <v>159</v>
+      </c>
+      <c r="K19" t="s">
+        <v>160</v>
+      </c>
+      <c r="L19" t="s">
+        <v>202</v>
+      </c>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="P19" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S19"/>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>203</v>
+      </c>
+      <c r="C20" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20" s="31" t="n">
+        <v>11579.0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>134</v>
+      </c>
+      <c r="G20" t="s">
+        <v>174</v>
+      </c>
+      <c r="H20" t="s">
+        <v>205</v>
+      </c>
+      <c r="I20" t="s">
+        <v>158</v>
+      </c>
+      <c r="J20" t="s">
+        <v>159</v>
+      </c>
+      <c r="K20" t="s">
+        <v>160</v>
+      </c>
+      <c r="L20" t="s">
+        <v>206</v>
+      </c>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="P20" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>134</v>
+      </c>
+      <c r="R20" t="s">
+        <v>166</v>
+      </c>
+      <c r="S20"/>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>207</v>
+      </c>
+      <c r="C21" t="s">
+        <v>208</v>
+      </c>
+      <c r="D21" s="32" t="n">
+        <v>10535.0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>134</v>
+      </c>
+      <c r="G21" t="s">
+        <v>156</v>
+      </c>
+      <c r="H21" t="s">
+        <v>209</v>
+      </c>
+      <c r="I21" t="s">
+        <v>158</v>
+      </c>
+      <c r="J21" t="s">
+        <v>159</v>
+      </c>
+      <c r="K21" t="s">
+        <v>160</v>
+      </c>
+      <c r="L21" t="s">
+        <v>210</v>
+      </c>
+      <c r="M21" t="s">
+        <v>211</v>
+      </c>
+      <c r="N21"/>
+      <c r="P21" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>134</v>
+      </c>
+      <c r="R21" t="s">
+        <v>166</v>
+      </c>
+      <c r="S21"/>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>213</v>
+      </c>
+      <c r="C22" t="s">
+        <v>214</v>
+      </c>
+      <c r="D22" s="33" t="n">
+        <v>15667.0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>134</v>
+      </c>
+      <c r="G22" t="s">
+        <v>156</v>
+      </c>
+      <c r="H22" t="s">
+        <v>215</v>
+      </c>
+      <c r="I22" t="s">
+        <v>158</v>
+      </c>
+      <c r="J22" t="s">
+        <v>159</v>
+      </c>
+      <c r="K22" t="s">
+        <v>160</v>
+      </c>
+      <c r="L22" t="s">
+        <v>216</v>
+      </c>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="P22" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>134</v>
+      </c>
+      <c r="R22" t="s">
+        <v>166</v>
+      </c>
+      <c r="S22"/>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>153</v>
+      </c>
+      <c r="C23" t="s">
+        <v>154</v>
+      </c>
+      <c r="D23" s="34" t="n">
+        <v>14198.0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>155</v>
+      </c>
+      <c r="G23" t="s">
+        <v>156</v>
+      </c>
+      <c r="H23" t="s">
+        <v>157</v>
+      </c>
+      <c r="I23" t="s">
+        <v>158</v>
+      </c>
+      <c r="J23" t="s">
+        <v>159</v>
+      </c>
+      <c r="K23" t="s">
+        <v>160</v>
+      </c>
+      <c r="L23" t="s">
+        <v>161</v>
+      </c>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="P23" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>134</v>
+      </c>
+      <c r="R23" t="s">
+        <v>134</v>
+      </c>
+      <c r="S23"/>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>162</v>
+      </c>
+      <c r="C24" t="s">
+        <v>163</v>
+      </c>
+      <c r="D24" s="35" t="n">
+        <v>15962.0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>134</v>
+      </c>
+      <c r="G24" t="s">
+        <v>156</v>
+      </c>
+      <c r="H24" t="s">
+        <v>164</v>
+      </c>
+      <c r="I24" t="s">
+        <v>158</v>
+      </c>
+      <c r="J24" t="s">
+        <v>159</v>
+      </c>
+      <c r="K24" t="s">
+        <v>160</v>
+      </c>
+      <c r="L24" t="s">
+        <v>165</v>
+      </c>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="P24" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>134</v>
+      </c>
+      <c r="R24" t="s">
+        <v>166</v>
+      </c>
+      <c r="S24"/>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25" t="s">
+        <v>168</v>
+      </c>
+      <c r="D25" s="36" t="n">
+        <v>13466.0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>155</v>
+      </c>
+      <c r="G25" t="s">
+        <v>156</v>
+      </c>
+      <c r="H25" t="s">
+        <v>169</v>
+      </c>
+      <c r="I25" t="s">
+        <v>158</v>
+      </c>
+      <c r="J25" t="s">
+        <v>159</v>
+      </c>
+      <c r="K25" t="s">
+        <v>160</v>
+      </c>
+      <c r="L25" t="s">
+        <v>170</v>
+      </c>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="P25" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>134</v>
+      </c>
+      <c r="R25" t="s">
+        <v>134</v>
+      </c>
+      <c r="S25"/>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>172</v>
+      </c>
+      <c r="C26" t="s">
+        <v>173</v>
+      </c>
+      <c r="D26" s="37" t="n">
+        <v>23463.0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>134</v>
+      </c>
+      <c r="G26" t="s">
+        <v>174</v>
+      </c>
+      <c r="H26" t="s">
+        <v>175</v>
+      </c>
+      <c r="I26" t="s">
+        <v>158</v>
+      </c>
+      <c r="J26" t="s">
+        <v>159</v>
+      </c>
+      <c r="K26" t="s">
+        <v>160</v>
+      </c>
+      <c r="L26" t="s">
+        <v>176</v>
+      </c>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="P26" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>134</v>
+      </c>
+      <c r="R26" t="s">
+        <v>166</v>
+      </c>
+      <c r="S26"/>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>178</v>
+      </c>
+      <c r="C27" t="s">
+        <v>179</v>
+      </c>
+      <c r="D27" s="38" t="n">
+        <v>11085.0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>134</v>
+      </c>
+      <c r="G27" t="s">
+        <v>156</v>
+      </c>
+      <c r="H27" t="s">
+        <v>180</v>
+      </c>
+      <c r="I27" t="s">
+        <v>158</v>
+      </c>
+      <c r="J27" t="s">
+        <v>159</v>
+      </c>
+      <c r="K27" t="s">
+        <v>160</v>
+      </c>
+      <c r="L27" t="s">
+        <v>181</v>
+      </c>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="P27" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>134</v>
+      </c>
+      <c r="R27" t="s">
+        <v>134</v>
+      </c>
+      <c r="S27"/>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C28" t="s">
+        <v>185</v>
+      </c>
+      <c r="D28" s="39" t="n">
+        <v>21738.0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>134</v>
+      </c>
+      <c r="G28" t="s">
+        <v>156</v>
+      </c>
+      <c r="H28" t="s">
+        <v>186</v>
+      </c>
+      <c r="I28" t="s">
+        <v>158</v>
+      </c>
+      <c r="J28" t="s">
+        <v>159</v>
+      </c>
+      <c r="K28" t="s">
+        <v>160</v>
+      </c>
+      <c r="L28" t="s">
+        <v>187</v>
+      </c>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="P28" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>134</v>
+      </c>
+      <c r="R28" t="s">
+        <v>166</v>
+      </c>
+      <c r="S28"/>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>189</v>
+      </c>
+      <c r="C29" t="s">
+        <v>190</v>
+      </c>
+      <c r="D29" s="40" t="n">
+        <v>9319.0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>134</v>
+      </c>
+      <c r="G29" t="s">
+        <v>156</v>
+      </c>
+      <c r="H29" t="s">
+        <v>191</v>
+      </c>
+      <c r="I29" t="s">
+        <v>158</v>
+      </c>
+      <c r="J29" t="s">
+        <v>159</v>
+      </c>
+      <c r="K29" t="s">
+        <v>160</v>
+      </c>
+      <c r="L29" t="s">
+        <v>192</v>
+      </c>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="P29" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>134</v>
+      </c>
+      <c r="R29" t="s">
+        <v>134</v>
+      </c>
+      <c r="S29"/>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
+        <v>193</v>
+      </c>
+      <c r="C30" t="s">
+        <v>194</v>
+      </c>
+      <c r="D30" s="41" t="n">
+        <v>21385.0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>134</v>
+      </c>
+      <c r="G30" t="s">
+        <v>156</v>
+      </c>
+      <c r="H30" t="s">
+        <v>195</v>
+      </c>
+      <c r="I30" t="s">
+        <v>158</v>
+      </c>
+      <c r="J30" t="s">
+        <v>159</v>
+      </c>
+      <c r="K30" t="s">
+        <v>160</v>
+      </c>
+      <c r="L30" t="s">
+        <v>196</v>
+      </c>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="P30" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>134</v>
+      </c>
+      <c r="R30" t="s">
+        <v>166</v>
+      </c>
+      <c r="S30"/>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>199</v>
+      </c>
+      <c r="C31" t="s">
+        <v>200</v>
+      </c>
+      <c r="D31" s="42" t="n">
+        <v>10690.0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>134</v>
+      </c>
+      <c r="G31" t="s">
+        <v>174</v>
+      </c>
+      <c r="H31" t="s">
+        <v>201</v>
+      </c>
+      <c r="I31" t="s">
+        <v>158</v>
+      </c>
+      <c r="J31" t="s">
+        <v>159</v>
+      </c>
+      <c r="K31" t="s">
+        <v>160</v>
+      </c>
+      <c r="L31" t="s">
+        <v>202</v>
+      </c>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="P31" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>134</v>
+      </c>
+      <c r="R31" t="s">
+        <v>134</v>
+      </c>
+      <c r="S31"/>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>203</v>
+      </c>
+      <c r="C32" t="s">
+        <v>204</v>
+      </c>
+      <c r="D32" s="43" t="n">
+        <v>11579.0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>134</v>
+      </c>
+      <c r="G32" t="s">
+        <v>174</v>
+      </c>
+      <c r="H32" t="s">
+        <v>205</v>
+      </c>
+      <c r="I32" t="s">
+        <v>158</v>
+      </c>
+      <c r="J32" t="s">
+        <v>159</v>
+      </c>
+      <c r="K32" t="s">
+        <v>160</v>
+      </c>
+      <c r="L32" t="s">
+        <v>206</v>
+      </c>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="P32" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>134</v>
+      </c>
+      <c r="R32" t="s">
+        <v>166</v>
+      </c>
+      <c r="S32"/>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>207</v>
+      </c>
+      <c r="C33" t="s">
+        <v>208</v>
+      </c>
+      <c r="D33" s="44" t="n">
+        <v>10535.0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>134</v>
+      </c>
+      <c r="G33" t="s">
+        <v>156</v>
+      </c>
+      <c r="H33" t="s">
+        <v>209</v>
+      </c>
+      <c r="I33" t="s">
+        <v>158</v>
+      </c>
+      <c r="J33" t="s">
+        <v>159</v>
+      </c>
+      <c r="K33" t="s">
+        <v>160</v>
+      </c>
+      <c r="L33" t="s">
+        <v>210</v>
+      </c>
+      <c r="M33" t="s">
+        <v>211</v>
+      </c>
+      <c r="N33"/>
+      <c r="P33" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>134</v>
+      </c>
+      <c r="R33" t="s">
+        <v>166</v>
+      </c>
+      <c r="S33"/>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>213</v>
+      </c>
+      <c r="C34" t="s">
+        <v>214</v>
+      </c>
+      <c r="D34" s="45" t="n">
+        <v>15667.0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>134</v>
+      </c>
+      <c r="G34" t="s">
+        <v>156</v>
+      </c>
+      <c r="H34" t="s">
+        <v>215</v>
+      </c>
+      <c r="I34" t="s">
+        <v>158</v>
+      </c>
+      <c r="J34" t="s">
+        <v>159</v>
+      </c>
+      <c r="K34" t="s">
+        <v>160</v>
+      </c>
+      <c r="L34" t="s">
+        <v>216</v>
+      </c>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="P34" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>134</v>
+      </c>
+      <c r="R34" t="s">
+        <v>166</v>
+      </c>
+      <c r="S34"/>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35" t="s">
+        <v>154</v>
+      </c>
+      <c r="D35" s="46" t="n">
+        <v>14198.0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>155</v>
+      </c>
+      <c r="G35" t="s">
+        <v>156</v>
+      </c>
+      <c r="H35" t="s">
+        <v>157</v>
+      </c>
+      <c r="I35" t="s">
+        <v>158</v>
+      </c>
+      <c r="J35" t="s">
+        <v>159</v>
+      </c>
+      <c r="K35" t="s">
+        <v>160</v>
+      </c>
+      <c r="L35" t="s">
+        <v>161</v>
+      </c>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="P35" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>134</v>
+      </c>
+      <c r="R35" t="s">
+        <v>134</v>
+      </c>
+      <c r="S35"/>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>162</v>
+      </c>
+      <c r="C36" t="s">
+        <v>163</v>
+      </c>
+      <c r="D36" s="47" t="n">
+        <v>15962.0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>134</v>
+      </c>
+      <c r="G36" t="s">
+        <v>156</v>
+      </c>
+      <c r="H36" t="s">
+        <v>164</v>
+      </c>
+      <c r="I36" t="s">
+        <v>158</v>
+      </c>
+      <c r="J36" t="s">
+        <v>159</v>
+      </c>
+      <c r="K36" t="s">
+        <v>160</v>
+      </c>
+      <c r="L36" t="s">
+        <v>165</v>
+      </c>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="P36" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>134</v>
+      </c>
+      <c r="R36" t="s">
+        <v>166</v>
+      </c>
+      <c r="S36"/>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>167</v>
+      </c>
+      <c r="C37" t="s">
+        <v>168</v>
+      </c>
+      <c r="D37" s="48" t="n">
+        <v>13466.0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>155</v>
+      </c>
+      <c r="G37" t="s">
+        <v>156</v>
+      </c>
+      <c r="H37" t="s">
+        <v>169</v>
+      </c>
+      <c r="I37" t="s">
+        <v>158</v>
+      </c>
+      <c r="J37" t="s">
+        <v>159</v>
+      </c>
+      <c r="K37" t="s">
+        <v>160</v>
+      </c>
+      <c r="L37" t="s">
+        <v>170</v>
+      </c>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="P37" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>134</v>
+      </c>
+      <c r="R37" t="s">
+        <v>134</v>
+      </c>
+      <c r="S37"/>
+    </row>
+    <row r="38">
+      <c r="B38" t="s">
+        <v>172</v>
+      </c>
+      <c r="C38" t="s">
+        <v>173</v>
+      </c>
+      <c r="D38" s="49" t="n">
+        <v>23463.0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>134</v>
+      </c>
+      <c r="G38" t="s">
+        <v>174</v>
+      </c>
+      <c r="H38" t="s">
+        <v>175</v>
+      </c>
+      <c r="I38" t="s">
+        <v>158</v>
+      </c>
+      <c r="J38" t="s">
+        <v>159</v>
+      </c>
+      <c r="K38" t="s">
+        <v>160</v>
+      </c>
+      <c r="L38" t="s">
+        <v>176</v>
+      </c>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="P38" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>134</v>
+      </c>
+      <c r="R38" t="s">
+        <v>166</v>
+      </c>
+      <c r="S38"/>
+    </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>178</v>
+      </c>
+      <c r="C39" t="s">
+        <v>179</v>
+      </c>
+      <c r="D39" s="50" t="n">
+        <v>11085.0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>134</v>
+      </c>
+      <c r="G39" t="s">
+        <v>156</v>
+      </c>
+      <c r="H39" t="s">
+        <v>180</v>
+      </c>
+      <c r="I39" t="s">
+        <v>158</v>
+      </c>
+      <c r="J39" t="s">
+        <v>159</v>
+      </c>
+      <c r="K39" t="s">
+        <v>160</v>
+      </c>
+      <c r="L39" t="s">
+        <v>181</v>
+      </c>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="P39" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>134</v>
+      </c>
+      <c r="R39" t="s">
+        <v>134</v>
+      </c>
+      <c r="S39"/>
+    </row>
+    <row r="40">
+      <c r="B40" t="s">
+        <v>184</v>
+      </c>
+      <c r="C40" t="s">
+        <v>185</v>
+      </c>
+      <c r="D40" s="51" t="n">
+        <v>21738.0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>134</v>
+      </c>
+      <c r="G40" t="s">
+        <v>156</v>
+      </c>
+      <c r="H40" t="s">
+        <v>186</v>
+      </c>
+      <c r="I40" t="s">
+        <v>158</v>
+      </c>
+      <c r="J40" t="s">
+        <v>159</v>
+      </c>
+      <c r="K40" t="s">
+        <v>160</v>
+      </c>
+      <c r="L40" t="s">
+        <v>187</v>
+      </c>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="P40" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>134</v>
+      </c>
+      <c r="R40" t="s">
+        <v>166</v>
+      </c>
+      <c r="S40"/>
+    </row>
+    <row r="41">
+      <c r="B41" t="s">
+        <v>189</v>
+      </c>
+      <c r="C41" t="s">
+        <v>190</v>
+      </c>
+      <c r="D41" s="52" t="n">
+        <v>9319.0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>134</v>
+      </c>
+      <c r="G41" t="s">
+        <v>156</v>
+      </c>
+      <c r="H41" t="s">
+        <v>191</v>
+      </c>
+      <c r="I41" t="s">
+        <v>158</v>
+      </c>
+      <c r="J41" t="s">
+        <v>159</v>
+      </c>
+      <c r="K41" t="s">
+        <v>160</v>
+      </c>
+      <c r="L41" t="s">
+        <v>192</v>
+      </c>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="P41" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>134</v>
+      </c>
+      <c r="R41" t="s">
+        <v>134</v>
+      </c>
+      <c r="S41"/>
+    </row>
+    <row r="42">
+      <c r="B42" t="s">
+        <v>193</v>
+      </c>
+      <c r="C42" t="s">
+        <v>194</v>
+      </c>
+      <c r="D42" s="53" t="n">
+        <v>21385.0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>134</v>
+      </c>
+      <c r="G42" t="s">
+        <v>156</v>
+      </c>
+      <c r="H42" t="s">
+        <v>195</v>
+      </c>
+      <c r="I42" t="s">
+        <v>158</v>
+      </c>
+      <c r="J42" t="s">
+        <v>159</v>
+      </c>
+      <c r="K42" t="s">
+        <v>160</v>
+      </c>
+      <c r="L42" t="s">
+        <v>196</v>
+      </c>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="P42" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>134</v>
+      </c>
+      <c r="R42" t="s">
+        <v>166</v>
+      </c>
+      <c r="S42"/>
+    </row>
+    <row r="43">
+      <c r="B43" t="s">
+        <v>199</v>
+      </c>
+      <c r="C43" t="s">
+        <v>200</v>
+      </c>
+      <c r="D43" s="54" t="n">
+        <v>10690.0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>134</v>
+      </c>
+      <c r="G43" t="s">
+        <v>174</v>
+      </c>
+      <c r="H43" t="s">
+        <v>201</v>
+      </c>
+      <c r="I43" t="s">
+        <v>158</v>
+      </c>
+      <c r="J43" t="s">
+        <v>159</v>
+      </c>
+      <c r="K43" t="s">
+        <v>160</v>
+      </c>
+      <c r="L43" t="s">
+        <v>202</v>
+      </c>
+      <c r="M43"/>
+      <c r="N43"/>
+      <c r="P43" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>134</v>
+      </c>
+      <c r="R43" t="s">
+        <v>134</v>
+      </c>
+      <c r="S43"/>
+    </row>
+    <row r="44">
+      <c r="B44" t="s">
+        <v>203</v>
+      </c>
+      <c r="C44" t="s">
+        <v>204</v>
+      </c>
+      <c r="D44" s="55" t="n">
+        <v>11579.0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>134</v>
+      </c>
+      <c r="G44" t="s">
+        <v>174</v>
+      </c>
+      <c r="H44" t="s">
+        <v>205</v>
+      </c>
+      <c r="I44" t="s">
+        <v>158</v>
+      </c>
+      <c r="J44" t="s">
+        <v>159</v>
+      </c>
+      <c r="K44" t="s">
+        <v>160</v>
+      </c>
+      <c r="L44" t="s">
+        <v>206</v>
+      </c>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="P44" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>134</v>
+      </c>
+      <c r="R44" t="s">
+        <v>166</v>
+      </c>
+      <c r="S44"/>
+    </row>
+    <row r="45">
+      <c r="B45" t="s">
+        <v>207</v>
+      </c>
+      <c r="C45" t="s">
+        <v>208</v>
+      </c>
+      <c r="D45" s="56" t="n">
+        <v>10535.0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>134</v>
+      </c>
+      <c r="G45" t="s">
+        <v>156</v>
+      </c>
+      <c r="H45" t="s">
+        <v>209</v>
+      </c>
+      <c r="I45" t="s">
+        <v>158</v>
+      </c>
+      <c r="J45" t="s">
+        <v>159</v>
+      </c>
+      <c r="K45" t="s">
+        <v>160</v>
+      </c>
+      <c r="L45" t="s">
+        <v>210</v>
+      </c>
+      <c r="M45" t="s">
+        <v>211</v>
+      </c>
+      <c r="N45"/>
+      <c r="P45" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>134</v>
+      </c>
+      <c r="R45" t="s">
+        <v>166</v>
+      </c>
+      <c r="S45"/>
+    </row>
+    <row r="46">
+      <c r="B46" t="s">
+        <v>213</v>
+      </c>
+      <c r="C46" t="s">
+        <v>214</v>
+      </c>
+      <c r="D46" s="57" t="n">
+        <v>15667.0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>134</v>
+      </c>
+      <c r="G46" t="s">
+        <v>156</v>
+      </c>
+      <c r="H46" t="s">
+        <v>215</v>
+      </c>
+      <c r="I46" t="s">
+        <v>158</v>
+      </c>
+      <c r="J46" t="s">
+        <v>159</v>
+      </c>
+      <c r="K46" t="s">
+        <v>160</v>
+      </c>
+      <c r="L46" t="s">
+        <v>216</v>
+      </c>
+      <c r="M46"/>
+      <c r="N46"/>
+      <c r="P46" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>134</v>
+      </c>
+      <c r="R46" t="s">
+        <v>166</v>
+      </c>
+      <c r="S46"/>
+    </row>
+    <row r="47">
+      <c r="B47" t="s">
+        <v>153</v>
+      </c>
+      <c r="C47" t="s">
+        <v>154</v>
+      </c>
+      <c r="D47" s="58" t="n">
+        <v>14198.0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>155</v>
+      </c>
+      <c r="G47" t="s">
+        <v>156</v>
+      </c>
+      <c r="H47" t="s">
+        <v>157</v>
+      </c>
+      <c r="I47" t="s">
+        <v>158</v>
+      </c>
+      <c r="J47" t="s">
+        <v>159</v>
+      </c>
+      <c r="K47" t="s">
+        <v>160</v>
+      </c>
+      <c r="L47" t="s">
+        <v>161</v>
+      </c>
+      <c r="M47"/>
+      <c r="N47"/>
+      <c r="P47" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>134</v>
+      </c>
+      <c r="R47" t="s">
+        <v>134</v>
+      </c>
+      <c r="S47"/>
+    </row>
+    <row r="48">
+      <c r="B48" t="s">
+        <v>162</v>
+      </c>
+      <c r="C48" t="s">
+        <v>163</v>
+      </c>
+      <c r="D48" s="59" t="n">
+        <v>15962.0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>134</v>
+      </c>
+      <c r="G48" t="s">
+        <v>156</v>
+      </c>
+      <c r="H48" t="s">
+        <v>164</v>
+      </c>
+      <c r="I48" t="s">
+        <v>158</v>
+      </c>
+      <c r="J48" t="s">
+        <v>159</v>
+      </c>
+      <c r="K48" t="s">
+        <v>160</v>
+      </c>
+      <c r="L48" t="s">
+        <v>165</v>
+      </c>
+      <c r="M48"/>
+      <c r="N48"/>
+      <c r="P48" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>134</v>
+      </c>
+      <c r="R48" t="s">
+        <v>166</v>
+      </c>
+      <c r="S48"/>
+    </row>
+    <row r="49">
+      <c r="B49" t="s">
+        <v>167</v>
+      </c>
+      <c r="C49" t="s">
+        <v>168</v>
+      </c>
+      <c r="D49" s="60" t="n">
+        <v>13466.0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>155</v>
+      </c>
+      <c r="G49" t="s">
+        <v>156</v>
+      </c>
+      <c r="H49" t="s">
+        <v>169</v>
+      </c>
+      <c r="I49" t="s">
+        <v>158</v>
+      </c>
+      <c r="J49" t="s">
+        <v>159</v>
+      </c>
+      <c r="K49" t="s">
+        <v>160</v>
+      </c>
+      <c r="L49" t="s">
+        <v>170</v>
+      </c>
+      <c r="M49"/>
+      <c r="N49"/>
+      <c r="P49" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>134</v>
+      </c>
+      <c r="R49" t="s">
+        <v>134</v>
+      </c>
+      <c r="S49"/>
+    </row>
+    <row r="50">
+      <c r="B50" t="s">
+        <v>172</v>
+      </c>
+      <c r="C50" t="s">
+        <v>173</v>
+      </c>
+      <c r="D50" s="61" t="n">
+        <v>23463.0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>134</v>
+      </c>
+      <c r="G50" t="s">
+        <v>174</v>
+      </c>
+      <c r="H50" t="s">
+        <v>175</v>
+      </c>
+      <c r="I50" t="s">
+        <v>158</v>
+      </c>
+      <c r="J50" t="s">
+        <v>159</v>
+      </c>
+      <c r="K50" t="s">
+        <v>160</v>
+      </c>
+      <c r="L50" t="s">
+        <v>176</v>
+      </c>
+      <c r="M50"/>
+      <c r="N50"/>
+      <c r="P50" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>134</v>
+      </c>
+      <c r="R50" t="s">
+        <v>166</v>
+      </c>
+      <c r="S50"/>
+    </row>
+    <row r="51">
+      <c r="B51" t="s">
+        <v>178</v>
+      </c>
+      <c r="C51" t="s">
+        <v>179</v>
+      </c>
+      <c r="D51" s="62" t="n">
+        <v>11085.0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>134</v>
+      </c>
+      <c r="G51" t="s">
+        <v>156</v>
+      </c>
+      <c r="H51" t="s">
+        <v>180</v>
+      </c>
+      <c r="I51" t="s">
+        <v>158</v>
+      </c>
+      <c r="J51" t="s">
+        <v>159</v>
+      </c>
+      <c r="K51" t="s">
+        <v>160</v>
+      </c>
+      <c r="L51" t="s">
+        <v>181</v>
+      </c>
+      <c r="M51"/>
+      <c r="N51"/>
+      <c r="P51" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>134</v>
+      </c>
+      <c r="R51" t="s">
+        <v>134</v>
+      </c>
+      <c r="S51"/>
+    </row>
+    <row r="52">
+      <c r="B52" t="s">
+        <v>184</v>
+      </c>
+      <c r="C52" t="s">
+        <v>185</v>
+      </c>
+      <c r="D52" s="63" t="n">
+        <v>21738.0</v>
+      </c>
+      <c r="F52" t="s">
+        <v>134</v>
+      </c>
+      <c r="G52" t="s">
+        <v>156</v>
+      </c>
+      <c r="H52" t="s">
+        <v>186</v>
+      </c>
+      <c r="I52" t="s">
+        <v>158</v>
+      </c>
+      <c r="J52" t="s">
+        <v>159</v>
+      </c>
+      <c r="K52" t="s">
+        <v>160</v>
+      </c>
+      <c r="L52" t="s">
+        <v>187</v>
+      </c>
+      <c r="M52"/>
+      <c r="N52"/>
+      <c r="P52" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>134</v>
+      </c>
+      <c r="R52" t="s">
+        <v>166</v>
+      </c>
+      <c r="S52"/>
+    </row>
+    <row r="53">
+      <c r="B53" t="s">
+        <v>189</v>
+      </c>
+      <c r="C53" t="s">
+        <v>190</v>
+      </c>
+      <c r="D53" s="64" t="n">
+        <v>9319.0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>134</v>
+      </c>
+      <c r="G53" t="s">
+        <v>156</v>
+      </c>
+      <c r="H53" t="s">
+        <v>191</v>
+      </c>
+      <c r="I53" t="s">
+        <v>158</v>
+      </c>
+      <c r="J53" t="s">
+        <v>159</v>
+      </c>
+      <c r="K53" t="s">
+        <v>160</v>
+      </c>
+      <c r="L53" t="s">
+        <v>192</v>
+      </c>
+      <c r="M53"/>
+      <c r="N53"/>
+      <c r="P53" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>134</v>
+      </c>
+      <c r="R53" t="s">
+        <v>134</v>
+      </c>
+      <c r="S53"/>
+    </row>
+    <row r="54">
+      <c r="B54" t="s">
+        <v>193</v>
+      </c>
+      <c r="C54" t="s">
+        <v>194</v>
+      </c>
+      <c r="D54" s="65" t="n">
+        <v>21385.0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>134</v>
+      </c>
+      <c r="G54" t="s">
+        <v>156</v>
+      </c>
+      <c r="H54" t="s">
+        <v>195</v>
+      </c>
+      <c r="I54" t="s">
+        <v>158</v>
+      </c>
+      <c r="J54" t="s">
+        <v>159</v>
+      </c>
+      <c r="K54" t="s">
+        <v>160</v>
+      </c>
+      <c r="L54" t="s">
+        <v>196</v>
+      </c>
+      <c r="M54"/>
+      <c r="N54"/>
+      <c r="P54" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>134</v>
+      </c>
+      <c r="R54" t="s">
+        <v>166</v>
+      </c>
+      <c r="S54"/>
+    </row>
+    <row r="55">
+      <c r="B55" t="s">
+        <v>199</v>
+      </c>
+      <c r="C55" t="s">
+        <v>200</v>
+      </c>
+      <c r="D55" s="66" t="n">
+        <v>10690.0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>134</v>
+      </c>
+      <c r="G55" t="s">
+        <v>174</v>
+      </c>
+      <c r="H55" t="s">
+        <v>201</v>
+      </c>
+      <c r="I55" t="s">
+        <v>158</v>
+      </c>
+      <c r="J55" t="s">
+        <v>159</v>
+      </c>
+      <c r="K55" t="s">
+        <v>160</v>
+      </c>
+      <c r="L55" t="s">
+        <v>202</v>
+      </c>
+      <c r="M55"/>
+      <c r="N55"/>
+      <c r="P55" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>134</v>
+      </c>
+      <c r="R55" t="s">
+        <v>134</v>
+      </c>
+      <c r="S55"/>
+    </row>
+    <row r="56">
+      <c r="B56" t="s">
+        <v>203</v>
+      </c>
+      <c r="C56" t="s">
+        <v>204</v>
+      </c>
+      <c r="D56" s="67" t="n">
+        <v>11579.0</v>
+      </c>
+      <c r="F56" t="s">
+        <v>134</v>
+      </c>
+      <c r="G56" t="s">
+        <v>174</v>
+      </c>
+      <c r="H56" t="s">
+        <v>205</v>
+      </c>
+      <c r="I56" t="s">
+        <v>158</v>
+      </c>
+      <c r="J56" t="s">
+        <v>159</v>
+      </c>
+      <c r="K56" t="s">
+        <v>160</v>
+      </c>
+      <c r="L56" t="s">
+        <v>206</v>
+      </c>
+      <c r="M56"/>
+      <c r="N56"/>
+      <c r="P56" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>134</v>
+      </c>
+      <c r="R56" t="s">
+        <v>166</v>
+      </c>
+      <c r="S56"/>
+    </row>
+    <row r="57">
+      <c r="B57" t="s">
+        <v>207</v>
+      </c>
+      <c r="C57" t="s">
+        <v>208</v>
+      </c>
+      <c r="D57" t="n" s="68">
+        <v>10535.0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>134</v>
+      </c>
+      <c r="G57" t="s">
+        <v>156</v>
+      </c>
+      <c r="H57" t="s">
+        <v>209</v>
+      </c>
+      <c r="I57" t="s">
+        <v>158</v>
+      </c>
+      <c r="J57" t="s">
+        <v>159</v>
+      </c>
+      <c r="K57" t="s">
+        <v>160</v>
+      </c>
+      <c r="L57" t="s">
+        <v>210</v>
+      </c>
+      <c r="M57" t="s">
+        <v>211</v>
+      </c>
+      <c r="N57"/>
+      <c r="P57" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>134</v>
+      </c>
+      <c r="R57" t="s">
+        <v>166</v>
+      </c>
+      <c r="S57"/>
+    </row>
   </sheetData>
   <dataConsolidate/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -1626,19 +3942,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'Referral Sheet'!$B$3:$B$30</xm:f>
           </x14:formula1>
           <xm:sqref>W4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'Current Studies'!$B$4:$B$11</xm:f>
           </x14:formula1>
           <xm:sqref>V4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>'Formulas&amp;Tables'!$G$5:$G$6</xm:f>
           </x14:formula1>
@@ -1651,9 +3967,9 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="B2:I9"/>
+  <dimension ref="B2:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
@@ -1661,8 +3977,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
@@ -1705,14 +4021,14 @@
       <c r="I9" s="6"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:AD7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B1:AE7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
@@ -1720,32 +4036,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="12" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="20" width="12" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="19.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="12" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="21.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="12" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="36.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="12" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="19.88671875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.88671875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="28.5546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="16" max="17" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="19" max="20" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="19.21875" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="36.77734375" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:30" x14ac:dyDescent="0.3">
@@ -2283,13 +4599,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B1:L8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="B1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
@@ -2297,7 +4613,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="12" width="11" customWidth="1" collapsed="1"/>
+    <col min="3" max="12" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.3">
@@ -2559,7 +4875,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -2567,7 +4883,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
             <xm:f>'Formulas&amp;Tables'!$G$4:$G$6</xm:f>
           </x14:formula1>
@@ -2580,8 +4896,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -2589,15 +4905,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="48.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="48.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="38.6640625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="23.88671875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.3">
@@ -2804,7 +5120,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -2812,8 +5128,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:AA8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B1:AB55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Z4" sqref="Z4"/>
@@ -2821,28 +5137,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="11.109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.5546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.6640625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="23.44140625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.6640625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="21" max="25" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="12.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="10.44140625" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="23.44140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="18" max="19" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="21" max="25" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="12.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15" r="1" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
@@ -3032,6 +5348,523 @@
       </c>
       <c r="D8" s="19">
         <v>25329</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="22" t="n">
+        <v>14198.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C10" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" s="23" t="n">
+        <v>15962.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" t="s">
+        <v>167</v>
+      </c>
+      <c r="D11" s="24" t="n">
+        <v>13466.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" t="s">
+        <v>172</v>
+      </c>
+      <c r="D12" s="25" t="n">
+        <v>23463.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>179</v>
+      </c>
+      <c r="C13" t="s">
+        <v>178</v>
+      </c>
+      <c r="D13" s="26" t="n">
+        <v>11085.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14" t="s">
+        <v>184</v>
+      </c>
+      <c r="D14" s="27" t="n">
+        <v>21738.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>190</v>
+      </c>
+      <c r="C15" t="s">
+        <v>189</v>
+      </c>
+      <c r="D15" s="28" t="n">
+        <v>9319.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C16" t="s">
+        <v>193</v>
+      </c>
+      <c r="D16" s="29" t="n">
+        <v>21385.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C17" t="s">
+        <v>199</v>
+      </c>
+      <c r="D17" s="30" t="n">
+        <v>10690.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C18" t="s">
+        <v>203</v>
+      </c>
+      <c r="D18" s="31" t="n">
+        <v>11579.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>208</v>
+      </c>
+      <c r="C19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D19" s="32" t="n">
+        <v>10535.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>214</v>
+      </c>
+      <c r="C20" t="s">
+        <v>213</v>
+      </c>
+      <c r="D20" s="33" t="n">
+        <v>15667.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>154</v>
+      </c>
+      <c r="C21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21" s="34" t="n">
+        <v>14198.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>163</v>
+      </c>
+      <c r="C22" t="s">
+        <v>162</v>
+      </c>
+      <c r="D22" s="35" t="n">
+        <v>15962.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>168</v>
+      </c>
+      <c r="C23" t="s">
+        <v>167</v>
+      </c>
+      <c r="D23" s="36" t="n">
+        <v>13466.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" s="37" t="n">
+        <v>23463.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" s="38" t="n">
+        <v>11085.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>185</v>
+      </c>
+      <c r="C26" t="s">
+        <v>184</v>
+      </c>
+      <c r="D26" s="39" t="n">
+        <v>21738.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>190</v>
+      </c>
+      <c r="C27" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" s="40" t="n">
+        <v>9319.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>194</v>
+      </c>
+      <c r="C28" t="s">
+        <v>193</v>
+      </c>
+      <c r="D28" s="41" t="n">
+        <v>21385.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>200</v>
+      </c>
+      <c r="C29" t="s">
+        <v>199</v>
+      </c>
+      <c r="D29" s="42" t="n">
+        <v>10690.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
+        <v>204</v>
+      </c>
+      <c r="C30" t="s">
+        <v>203</v>
+      </c>
+      <c r="D30" s="43" t="n">
+        <v>11579.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C31" t="s">
+        <v>207</v>
+      </c>
+      <c r="D31" s="44" t="n">
+        <v>10535.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>214</v>
+      </c>
+      <c r="C32" t="s">
+        <v>213</v>
+      </c>
+      <c r="D32" s="45" t="n">
+        <v>15667.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33" t="s">
+        <v>153</v>
+      </c>
+      <c r="D33" s="46" t="n">
+        <v>14198.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" t="s">
+        <v>162</v>
+      </c>
+      <c r="D34" s="47" t="n">
+        <v>15962.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>168</v>
+      </c>
+      <c r="C35" t="s">
+        <v>167</v>
+      </c>
+      <c r="D35" s="48" t="n">
+        <v>13466.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C36" t="s">
+        <v>172</v>
+      </c>
+      <c r="D36" s="49" t="n">
+        <v>23463.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>179</v>
+      </c>
+      <c r="C37" t="s">
+        <v>178</v>
+      </c>
+      <c r="D37" s="50" t="n">
+        <v>11085.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s">
+        <v>185</v>
+      </c>
+      <c r="C38" t="s">
+        <v>184</v>
+      </c>
+      <c r="D38" s="51" t="n">
+        <v>21738.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>190</v>
+      </c>
+      <c r="C39" t="s">
+        <v>189</v>
+      </c>
+      <c r="D39" s="52" t="n">
+        <v>9319.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="s">
+        <v>194</v>
+      </c>
+      <c r="C40" t="s">
+        <v>193</v>
+      </c>
+      <c r="D40" s="53" t="n">
+        <v>21385.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="s">
+        <v>200</v>
+      </c>
+      <c r="C41" t="s">
+        <v>199</v>
+      </c>
+      <c r="D41" s="54" t="n">
+        <v>10690.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s">
+        <v>204</v>
+      </c>
+      <c r="C42" t="s">
+        <v>203</v>
+      </c>
+      <c r="D42" s="55" t="n">
+        <v>11579.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s">
+        <v>208</v>
+      </c>
+      <c r="C43" t="s">
+        <v>207</v>
+      </c>
+      <c r="D43" s="56" t="n">
+        <v>10535.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="s">
+        <v>214</v>
+      </c>
+      <c r="C44" t="s">
+        <v>213</v>
+      </c>
+      <c r="D44" s="57" t="n">
+        <v>15667.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="s">
+        <v>154</v>
+      </c>
+      <c r="C45" t="s">
+        <v>153</v>
+      </c>
+      <c r="D45" s="58" t="n">
+        <v>14198.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="s">
+        <v>163</v>
+      </c>
+      <c r="C46" t="s">
+        <v>162</v>
+      </c>
+      <c r="D46" s="59" t="n">
+        <v>15962.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="s">
+        <v>168</v>
+      </c>
+      <c r="C47" t="s">
+        <v>167</v>
+      </c>
+      <c r="D47" s="60" t="n">
+        <v>13466.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="s">
+        <v>173</v>
+      </c>
+      <c r="C48" t="s">
+        <v>172</v>
+      </c>
+      <c r="D48" s="61" t="n">
+        <v>23463.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="s">
+        <v>179</v>
+      </c>
+      <c r="C49" t="s">
+        <v>178</v>
+      </c>
+      <c r="D49" s="62" t="n">
+        <v>11085.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="s">
+        <v>185</v>
+      </c>
+      <c r="C50" t="s">
+        <v>184</v>
+      </c>
+      <c r="D50" s="63" t="n">
+        <v>21738.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="s">
+        <v>190</v>
+      </c>
+      <c r="C51" t="s">
+        <v>189</v>
+      </c>
+      <c r="D51" s="64" t="n">
+        <v>9319.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="s">
+        <v>194</v>
+      </c>
+      <c r="C52" t="s">
+        <v>193</v>
+      </c>
+      <c r="D52" s="65" t="n">
+        <v>21385.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="s">
+        <v>200</v>
+      </c>
+      <c r="C53" t="s">
+        <v>199</v>
+      </c>
+      <c r="D53" s="66" t="n">
+        <v>10690.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="s">
+        <v>204</v>
+      </c>
+      <c r="C54" t="s">
+        <v>203</v>
+      </c>
+      <c r="D54" s="67" t="n">
+        <v>11579.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="s">
+        <v>208</v>
+      </c>
+      <c r="C55" t="s">
+        <v>207</v>
+      </c>
+      <c r="D55" t="n" s="68">
+        <v>10535.0</v>
       </c>
     </row>
   </sheetData>
@@ -3054,18 +5887,18 @@
     <mergeCell ref="Y1:Z1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="Z3:Z8" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation allowBlank="1" sqref="Z3:Z8" type="list" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>termReason</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:L2"/>
+  <dimension ref="B1:M49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
@@ -3073,14 +5906,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="14.4" r="1" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
@@ -3135,6 +5968,807 @@
       <c r="L2" s="13" t="s">
         <v>118</v>
       </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="22" t="n">
+        <v>14198.0</v>
+      </c>
+      <c r="E3" s="22"/>
+      <c r="F3"/>
+      <c r="G3" s="22"/>
+      <c r="H3"/>
+    </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="23" t="n">
+        <v>15962.0</v>
+      </c>
+      <c r="E4" s="23" t="n">
+        <v>42584.0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" s="23"/>
+      <c r="H4"/>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="24" t="n">
+        <v>13466.0</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5"/>
+      <c r="G5" s="24"/>
+      <c r="H5"/>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D6" s="25" t="n">
+        <v>23463.0</v>
+      </c>
+      <c r="E6" s="25"/>
+      <c r="F6"/>
+      <c r="G6" s="25" t="n">
+        <v>42923.0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D7" s="26" t="n">
+        <v>11085.0</v>
+      </c>
+      <c r="E7" s="26" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>183</v>
+      </c>
+      <c r="G7" s="26"/>
+      <c r="H7"/>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" s="27" t="n">
+        <v>21738.0</v>
+      </c>
+      <c r="E8" s="27" t="n">
+        <v>42856.0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G8" s="27"/>
+      <c r="H8"/>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D9" s="28" t="n">
+        <v>9319.0</v>
+      </c>
+      <c r="E9" s="28"/>
+      <c r="F9"/>
+      <c r="G9" s="28"/>
+      <c r="H9"/>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C10" t="s">
+        <v>193</v>
+      </c>
+      <c r="D10" s="29" t="n">
+        <v>21385.0</v>
+      </c>
+      <c r="E10" s="29" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>198</v>
+      </c>
+      <c r="G10" s="29"/>
+      <c r="H10"/>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" s="30" t="n">
+        <v>10690.0</v>
+      </c>
+      <c r="E11" s="30"/>
+      <c r="F11"/>
+      <c r="G11" s="30"/>
+      <c r="H11"/>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C12" t="s">
+        <v>203</v>
+      </c>
+      <c r="D12" s="31" t="n">
+        <v>11579.0</v>
+      </c>
+      <c r="E12" s="31"/>
+      <c r="F12"/>
+      <c r="G12" s="31"/>
+      <c r="H12"/>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>208</v>
+      </c>
+      <c r="C13" t="s">
+        <v>207</v>
+      </c>
+      <c r="D13" s="32" t="n">
+        <v>10535.0</v>
+      </c>
+      <c r="E13" s="32" t="n">
+        <v>42678.0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>212</v>
+      </c>
+      <c r="G13" s="32"/>
+      <c r="H13"/>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>214</v>
+      </c>
+      <c r="C14" t="s">
+        <v>213</v>
+      </c>
+      <c r="D14" s="33" t="n">
+        <v>15667.0</v>
+      </c>
+      <c r="E14" s="33"/>
+      <c r="F14"/>
+      <c r="G14" s="33"/>
+      <c r="H14"/>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" s="34" t="n">
+        <v>14198.0</v>
+      </c>
+      <c r="E15" s="34"/>
+      <c r="F15"/>
+      <c r="G15" s="34"/>
+      <c r="H15"/>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D16" s="35" t="n">
+        <v>15962.0</v>
+      </c>
+      <c r="E16" s="35" t="n">
+        <v>42584.0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>138</v>
+      </c>
+      <c r="G16" s="35"/>
+      <c r="H16"/>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>168</v>
+      </c>
+      <c r="C17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D17" s="36" t="n">
+        <v>13466.0</v>
+      </c>
+      <c r="E17" s="36"/>
+      <c r="F17"/>
+      <c r="G17" s="36"/>
+      <c r="H17"/>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D18" s="37" t="n">
+        <v>23463.0</v>
+      </c>
+      <c r="E18" s="37"/>
+      <c r="F18"/>
+      <c r="G18" s="37" t="n">
+        <v>42923.0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C19" t="s">
+        <v>178</v>
+      </c>
+      <c r="D19" s="38" t="n">
+        <v>11085.0</v>
+      </c>
+      <c r="E19" s="38" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>183</v>
+      </c>
+      <c r="G19" s="38"/>
+      <c r="H19"/>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>185</v>
+      </c>
+      <c r="C20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D20" s="39" t="n">
+        <v>21738.0</v>
+      </c>
+      <c r="E20" s="39" t="n">
+        <v>42856.0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>138</v>
+      </c>
+      <c r="G20" s="39"/>
+      <c r="H20"/>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>190</v>
+      </c>
+      <c r="C21" t="s">
+        <v>189</v>
+      </c>
+      <c r="D21" s="40" t="n">
+        <v>9319.0</v>
+      </c>
+      <c r="E21" s="40"/>
+      <c r="F21"/>
+      <c r="G21" s="40"/>
+      <c r="H21"/>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>194</v>
+      </c>
+      <c r="C22" t="s">
+        <v>193</v>
+      </c>
+      <c r="D22" s="41" t="n">
+        <v>21385.0</v>
+      </c>
+      <c r="E22" s="41" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>198</v>
+      </c>
+      <c r="G22" s="41"/>
+      <c r="H22"/>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>200</v>
+      </c>
+      <c r="C23" t="s">
+        <v>199</v>
+      </c>
+      <c r="D23" s="42" t="n">
+        <v>10690.0</v>
+      </c>
+      <c r="E23" s="42"/>
+      <c r="F23"/>
+      <c r="G23" s="42"/>
+      <c r="H23"/>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>204</v>
+      </c>
+      <c r="C24" t="s">
+        <v>203</v>
+      </c>
+      <c r="D24" s="43" t="n">
+        <v>11579.0</v>
+      </c>
+      <c r="E24" s="43"/>
+      <c r="F24"/>
+      <c r="G24" s="43"/>
+      <c r="H24"/>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>208</v>
+      </c>
+      <c r="C25" t="s">
+        <v>207</v>
+      </c>
+      <c r="D25" s="44" t="n">
+        <v>10535.0</v>
+      </c>
+      <c r="E25" s="44" t="n">
+        <v>42678.0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>212</v>
+      </c>
+      <c r="G25" s="44"/>
+      <c r="H25"/>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>214</v>
+      </c>
+      <c r="C26" t="s">
+        <v>213</v>
+      </c>
+      <c r="D26" s="45" t="n">
+        <v>15667.0</v>
+      </c>
+      <c r="E26" s="45"/>
+      <c r="F26"/>
+      <c r="G26" s="45"/>
+      <c r="H26"/>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" t="s">
+        <v>153</v>
+      </c>
+      <c r="D27" s="46" t="n">
+        <v>14198.0</v>
+      </c>
+      <c r="E27" s="46"/>
+      <c r="F27"/>
+      <c r="G27" s="46"/>
+      <c r="H27"/>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>163</v>
+      </c>
+      <c r="C28" t="s">
+        <v>162</v>
+      </c>
+      <c r="D28" s="47" t="n">
+        <v>15962.0</v>
+      </c>
+      <c r="E28" s="47" t="n">
+        <v>42584.0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>138</v>
+      </c>
+      <c r="G28" s="47"/>
+      <c r="H28"/>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C29" t="s">
+        <v>167</v>
+      </c>
+      <c r="D29" s="48" t="n">
+        <v>13466.0</v>
+      </c>
+      <c r="E29" s="48"/>
+      <c r="F29"/>
+      <c r="G29" s="48"/>
+      <c r="H29"/>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
+        <v>173</v>
+      </c>
+      <c r="C30" t="s">
+        <v>172</v>
+      </c>
+      <c r="D30" s="49" t="n">
+        <v>23463.0</v>
+      </c>
+      <c r="E30" s="49"/>
+      <c r="F30"/>
+      <c r="G30" s="49" t="n">
+        <v>42923.0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>179</v>
+      </c>
+      <c r="C31" t="s">
+        <v>178</v>
+      </c>
+      <c r="D31" s="50" t="n">
+        <v>11085.0</v>
+      </c>
+      <c r="E31" s="50" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>183</v>
+      </c>
+      <c r="G31" s="50"/>
+      <c r="H31"/>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>185</v>
+      </c>
+      <c r="C32" t="s">
+        <v>184</v>
+      </c>
+      <c r="D32" s="51" t="n">
+        <v>21738.0</v>
+      </c>
+      <c r="E32" s="51" t="n">
+        <v>42856.0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>138</v>
+      </c>
+      <c r="G32" s="51"/>
+      <c r="H32"/>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>190</v>
+      </c>
+      <c r="C33" t="s">
+        <v>189</v>
+      </c>
+      <c r="D33" s="52" t="n">
+        <v>9319.0</v>
+      </c>
+      <c r="E33" s="52"/>
+      <c r="F33"/>
+      <c r="G33" s="52"/>
+      <c r="H33"/>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>194</v>
+      </c>
+      <c r="C34" t="s">
+        <v>193</v>
+      </c>
+      <c r="D34" s="53" t="n">
+        <v>21385.0</v>
+      </c>
+      <c r="E34" s="53" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>198</v>
+      </c>
+      <c r="G34" s="53"/>
+      <c r="H34"/>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>200</v>
+      </c>
+      <c r="C35" t="s">
+        <v>199</v>
+      </c>
+      <c r="D35" s="54" t="n">
+        <v>10690.0</v>
+      </c>
+      <c r="E35" s="54"/>
+      <c r="F35"/>
+      <c r="G35" s="54"/>
+      <c r="H35"/>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>204</v>
+      </c>
+      <c r="C36" t="s">
+        <v>203</v>
+      </c>
+      <c r="D36" s="55" t="n">
+        <v>11579.0</v>
+      </c>
+      <c r="E36" s="55"/>
+      <c r="F36"/>
+      <c r="G36" s="55"/>
+      <c r="H36"/>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>208</v>
+      </c>
+      <c r="C37" t="s">
+        <v>207</v>
+      </c>
+      <c r="D37" s="56" t="n">
+        <v>10535.0</v>
+      </c>
+      <c r="E37" s="56" t="n">
+        <v>42678.0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>212</v>
+      </c>
+      <c r="G37" s="56"/>
+      <c r="H37"/>
+    </row>
+    <row r="38">
+      <c r="B38" t="s">
+        <v>214</v>
+      </c>
+      <c r="C38" t="s">
+        <v>213</v>
+      </c>
+      <c r="D38" s="57" t="n">
+        <v>15667.0</v>
+      </c>
+      <c r="E38" s="57"/>
+      <c r="F38"/>
+      <c r="G38" s="57"/>
+      <c r="H38"/>
+    </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>154</v>
+      </c>
+      <c r="C39" t="s">
+        <v>153</v>
+      </c>
+      <c r="D39" s="58" t="n">
+        <v>14198.0</v>
+      </c>
+      <c r="E39" s="58"/>
+      <c r="F39"/>
+      <c r="G39" s="58"/>
+      <c r="H39"/>
+    </row>
+    <row r="40">
+      <c r="B40" t="s">
+        <v>163</v>
+      </c>
+      <c r="C40" t="s">
+        <v>162</v>
+      </c>
+      <c r="D40" s="59" t="n">
+        <v>15962.0</v>
+      </c>
+      <c r="E40" s="59" t="n">
+        <v>42584.0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>138</v>
+      </c>
+      <c r="G40" s="59"/>
+      <c r="H40"/>
+    </row>
+    <row r="41">
+      <c r="B41" t="s">
+        <v>168</v>
+      </c>
+      <c r="C41" t="s">
+        <v>167</v>
+      </c>
+      <c r="D41" s="60" t="n">
+        <v>13466.0</v>
+      </c>
+      <c r="E41" s="60"/>
+      <c r="F41"/>
+      <c r="G41" s="60"/>
+      <c r="H41"/>
+    </row>
+    <row r="42">
+      <c r="B42" t="s">
+        <v>173</v>
+      </c>
+      <c r="C42" t="s">
+        <v>172</v>
+      </c>
+      <c r="D42" s="61" t="n">
+        <v>23463.0</v>
+      </c>
+      <c r="E42" s="61"/>
+      <c r="F42"/>
+      <c r="G42" s="61" t="n">
+        <v>42923.0</v>
+      </c>
+      <c r="H42" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s">
+        <v>179</v>
+      </c>
+      <c r="C43" t="s">
+        <v>178</v>
+      </c>
+      <c r="D43" s="62" t="n">
+        <v>11085.0</v>
+      </c>
+      <c r="E43" s="62" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>183</v>
+      </c>
+      <c r="G43" s="62"/>
+      <c r="H43"/>
+    </row>
+    <row r="44">
+      <c r="B44" t="s">
+        <v>185</v>
+      </c>
+      <c r="C44" t="s">
+        <v>184</v>
+      </c>
+      <c r="D44" s="63" t="n">
+        <v>21738.0</v>
+      </c>
+      <c r="E44" s="63" t="n">
+        <v>42856.0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>138</v>
+      </c>
+      <c r="G44" s="63"/>
+      <c r="H44"/>
+    </row>
+    <row r="45">
+      <c r="B45" t="s">
+        <v>190</v>
+      </c>
+      <c r="C45" t="s">
+        <v>189</v>
+      </c>
+      <c r="D45" s="64" t="n">
+        <v>9319.0</v>
+      </c>
+      <c r="E45" s="64"/>
+      <c r="F45"/>
+      <c r="G45" s="64"/>
+      <c r="H45"/>
+    </row>
+    <row r="46">
+      <c r="B46" t="s">
+        <v>194</v>
+      </c>
+      <c r="C46" t="s">
+        <v>193</v>
+      </c>
+      <c r="D46" s="65" t="n">
+        <v>21385.0</v>
+      </c>
+      <c r="E46" s="65" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>198</v>
+      </c>
+      <c r="G46" s="65"/>
+      <c r="H46"/>
+    </row>
+    <row r="47">
+      <c r="B47" t="s">
+        <v>200</v>
+      </c>
+      <c r="C47" t="s">
+        <v>199</v>
+      </c>
+      <c r="D47" s="66" t="n">
+        <v>10690.0</v>
+      </c>
+      <c r="E47" s="66"/>
+      <c r="F47"/>
+      <c r="G47" s="66"/>
+      <c r="H47"/>
+    </row>
+    <row r="48">
+      <c r="B48" t="s">
+        <v>204</v>
+      </c>
+      <c r="C48" t="s">
+        <v>203</v>
+      </c>
+      <c r="D48" s="67" t="n">
+        <v>11579.0</v>
+      </c>
+      <c r="E48" s="67"/>
+      <c r="F48"/>
+      <c r="G48" s="67"/>
+      <c r="H48"/>
+    </row>
+    <row r="49">
+      <c r="B49" t="s">
+        <v>208</v>
+      </c>
+      <c r="C49" t="s">
+        <v>207</v>
+      </c>
+      <c r="D49" t="n" s="68">
+        <v>10535.0</v>
+      </c>
+      <c r="E49" t="n" s="68">
+        <v>42678.0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>212</v>
+      </c>
+      <c r="G49" s="68"/>
+      <c r="H49"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3146,14 +6780,14 @@
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B2:D30"/>
+  <dimension ref="B2:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J38" sqref="J38"/>
@@ -3161,7 +6795,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
@@ -3314,7 +6948,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -3322,8 +6956,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="B2:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
@@ -3331,7 +6965,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="25.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
@@ -3380,7 +7014,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -3388,9 +7022,9 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="B2"/>
+  <dimension ref="B2:C2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
@@ -3398,7 +7032,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="14.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
@@ -3407,7 +7041,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
Added variables for parsed status
</commit_message>
<xml_diff>
--- a/RoperALZDataMigration/RoperSpreadSheet2.xlsx
+++ b/RoperALZDataMigration/RoperSpreadSheet2.xlsx
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="217">
   <si>
     <t>Last Name</t>
   </si>
@@ -828,7 +828,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="80">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
@@ -865,6 +865,17 @@
     <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
@@ -1357,7 +1368,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:Y57"/>
+  <dimension ref="B1:Y68"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
@@ -3893,7 +3904,7 @@
       <c r="C57" t="s">
         <v>208</v>
       </c>
-      <c r="D57" t="n" s="68">
+      <c r="D57" s="68" t="n">
         <v>10535.0</v>
       </c>
       <c r="F57" t="s">
@@ -3931,6 +3942,492 @@
         <v>166</v>
       </c>
       <c r="S57"/>
+    </row>
+    <row r="58">
+      <c r="B58" t="s">
+        <v>153</v>
+      </c>
+      <c r="C58" t="s">
+        <v>154</v>
+      </c>
+      <c r="D58" s="69" t="n">
+        <v>14198.0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>155</v>
+      </c>
+      <c r="G58" t="s">
+        <v>156</v>
+      </c>
+      <c r="H58" t="s">
+        <v>157</v>
+      </c>
+      <c r="I58" t="s">
+        <v>158</v>
+      </c>
+      <c r="J58" t="s">
+        <v>159</v>
+      </c>
+      <c r="K58" t="s">
+        <v>160</v>
+      </c>
+      <c r="L58" t="s">
+        <v>161</v>
+      </c>
+      <c r="M58"/>
+      <c r="N58"/>
+      <c r="P58" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>134</v>
+      </c>
+      <c r="R58" t="s">
+        <v>134</v>
+      </c>
+      <c r="S58"/>
+    </row>
+    <row r="59">
+      <c r="B59" t="s">
+        <v>162</v>
+      </c>
+      <c r="C59" t="s">
+        <v>163</v>
+      </c>
+      <c r="D59" s="70" t="n">
+        <v>15962.0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>134</v>
+      </c>
+      <c r="G59" t="s">
+        <v>156</v>
+      </c>
+      <c r="H59" t="s">
+        <v>164</v>
+      </c>
+      <c r="I59" t="s">
+        <v>158</v>
+      </c>
+      <c r="J59" t="s">
+        <v>159</v>
+      </c>
+      <c r="K59" t="s">
+        <v>160</v>
+      </c>
+      <c r="L59" t="s">
+        <v>165</v>
+      </c>
+      <c r="M59"/>
+      <c r="N59"/>
+      <c r="P59" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>134</v>
+      </c>
+      <c r="R59" t="s">
+        <v>166</v>
+      </c>
+      <c r="S59"/>
+    </row>
+    <row r="60">
+      <c r="B60" t="s">
+        <v>167</v>
+      </c>
+      <c r="C60" t="s">
+        <v>168</v>
+      </c>
+      <c r="D60" s="71" t="n">
+        <v>13466.0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>155</v>
+      </c>
+      <c r="G60" t="s">
+        <v>156</v>
+      </c>
+      <c r="H60" t="s">
+        <v>169</v>
+      </c>
+      <c r="I60" t="s">
+        <v>158</v>
+      </c>
+      <c r="J60" t="s">
+        <v>159</v>
+      </c>
+      <c r="K60" t="s">
+        <v>160</v>
+      </c>
+      <c r="L60" t="s">
+        <v>170</v>
+      </c>
+      <c r="M60"/>
+      <c r="N60"/>
+      <c r="P60" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>134</v>
+      </c>
+      <c r="R60" t="s">
+        <v>134</v>
+      </c>
+      <c r="S60"/>
+    </row>
+    <row r="61">
+      <c r="B61" t="s">
+        <v>172</v>
+      </c>
+      <c r="C61" t="s">
+        <v>173</v>
+      </c>
+      <c r="D61" s="72" t="n">
+        <v>23463.0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>134</v>
+      </c>
+      <c r="G61" t="s">
+        <v>174</v>
+      </c>
+      <c r="H61" t="s">
+        <v>175</v>
+      </c>
+      <c r="I61" t="s">
+        <v>158</v>
+      </c>
+      <c r="J61" t="s">
+        <v>159</v>
+      </c>
+      <c r="K61" t="s">
+        <v>160</v>
+      </c>
+      <c r="L61" t="s">
+        <v>176</v>
+      </c>
+      <c r="M61"/>
+      <c r="N61"/>
+      <c r="P61" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>134</v>
+      </c>
+      <c r="R61" t="s">
+        <v>166</v>
+      </c>
+      <c r="S61"/>
+    </row>
+    <row r="62">
+      <c r="B62" t="s">
+        <v>178</v>
+      </c>
+      <c r="C62" t="s">
+        <v>179</v>
+      </c>
+      <c r="D62" s="73" t="n">
+        <v>11085.0</v>
+      </c>
+      <c r="F62" t="s">
+        <v>134</v>
+      </c>
+      <c r="G62" t="s">
+        <v>156</v>
+      </c>
+      <c r="H62" t="s">
+        <v>180</v>
+      </c>
+      <c r="I62" t="s">
+        <v>158</v>
+      </c>
+      <c r="J62" t="s">
+        <v>159</v>
+      </c>
+      <c r="K62" t="s">
+        <v>160</v>
+      </c>
+      <c r="L62" t="s">
+        <v>181</v>
+      </c>
+      <c r="M62"/>
+      <c r="N62"/>
+      <c r="P62" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>134</v>
+      </c>
+      <c r="R62" t="s">
+        <v>134</v>
+      </c>
+      <c r="S62"/>
+    </row>
+    <row r="63">
+      <c r="B63" t="s">
+        <v>184</v>
+      </c>
+      <c r="C63" t="s">
+        <v>185</v>
+      </c>
+      <c r="D63" s="74" t="n">
+        <v>21738.0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>134</v>
+      </c>
+      <c r="G63" t="s">
+        <v>156</v>
+      </c>
+      <c r="H63" t="s">
+        <v>186</v>
+      </c>
+      <c r="I63" t="s">
+        <v>158</v>
+      </c>
+      <c r="J63" t="s">
+        <v>159</v>
+      </c>
+      <c r="K63" t="s">
+        <v>160</v>
+      </c>
+      <c r="L63" t="s">
+        <v>187</v>
+      </c>
+      <c r="M63"/>
+      <c r="N63"/>
+      <c r="P63" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>134</v>
+      </c>
+      <c r="R63" t="s">
+        <v>166</v>
+      </c>
+      <c r="S63"/>
+    </row>
+    <row r="64">
+      <c r="B64" t="s">
+        <v>189</v>
+      </c>
+      <c r="C64" t="s">
+        <v>190</v>
+      </c>
+      <c r="D64" s="75" t="n">
+        <v>9319.0</v>
+      </c>
+      <c r="F64" t="s">
+        <v>134</v>
+      </c>
+      <c r="G64" t="s">
+        <v>156</v>
+      </c>
+      <c r="H64" t="s">
+        <v>191</v>
+      </c>
+      <c r="I64" t="s">
+        <v>158</v>
+      </c>
+      <c r="J64" t="s">
+        <v>159</v>
+      </c>
+      <c r="K64" t="s">
+        <v>160</v>
+      </c>
+      <c r="L64" t="s">
+        <v>192</v>
+      </c>
+      <c r="M64"/>
+      <c r="N64"/>
+      <c r="P64" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>134</v>
+      </c>
+      <c r="R64" t="s">
+        <v>134</v>
+      </c>
+      <c r="S64"/>
+    </row>
+    <row r="65">
+      <c r="B65" t="s">
+        <v>193</v>
+      </c>
+      <c r="C65" t="s">
+        <v>194</v>
+      </c>
+      <c r="D65" s="76" t="n">
+        <v>21385.0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>134</v>
+      </c>
+      <c r="G65" t="s">
+        <v>156</v>
+      </c>
+      <c r="H65" t="s">
+        <v>195</v>
+      </c>
+      <c r="I65" t="s">
+        <v>158</v>
+      </c>
+      <c r="J65" t="s">
+        <v>159</v>
+      </c>
+      <c r="K65" t="s">
+        <v>160</v>
+      </c>
+      <c r="L65" t="s">
+        <v>196</v>
+      </c>
+      <c r="M65"/>
+      <c r="N65"/>
+      <c r="P65" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>134</v>
+      </c>
+      <c r="R65" t="s">
+        <v>166</v>
+      </c>
+      <c r="S65"/>
+    </row>
+    <row r="66">
+      <c r="B66" t="s">
+        <v>199</v>
+      </c>
+      <c r="C66" t="s">
+        <v>200</v>
+      </c>
+      <c r="D66" s="77" t="n">
+        <v>10690.0</v>
+      </c>
+      <c r="F66" t="s">
+        <v>134</v>
+      </c>
+      <c r="G66" t="s">
+        <v>174</v>
+      </c>
+      <c r="H66" t="s">
+        <v>201</v>
+      </c>
+      <c r="I66" t="s">
+        <v>158</v>
+      </c>
+      <c r="J66" t="s">
+        <v>159</v>
+      </c>
+      <c r="K66" t="s">
+        <v>160</v>
+      </c>
+      <c r="L66" t="s">
+        <v>202</v>
+      </c>
+      <c r="M66"/>
+      <c r="N66"/>
+      <c r="P66" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>134</v>
+      </c>
+      <c r="R66" t="s">
+        <v>134</v>
+      </c>
+      <c r="S66"/>
+    </row>
+    <row r="67">
+      <c r="B67" t="s">
+        <v>203</v>
+      </c>
+      <c r="C67" t="s">
+        <v>204</v>
+      </c>
+      <c r="D67" s="78" t="n">
+        <v>11579.0</v>
+      </c>
+      <c r="F67" t="s">
+        <v>134</v>
+      </c>
+      <c r="G67" t="s">
+        <v>174</v>
+      </c>
+      <c r="H67" t="s">
+        <v>205</v>
+      </c>
+      <c r="I67" t="s">
+        <v>158</v>
+      </c>
+      <c r="J67" t="s">
+        <v>159</v>
+      </c>
+      <c r="K67" t="s">
+        <v>160</v>
+      </c>
+      <c r="L67" t="s">
+        <v>206</v>
+      </c>
+      <c r="M67"/>
+      <c r="N67"/>
+      <c r="P67" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>134</v>
+      </c>
+      <c r="R67" t="s">
+        <v>166</v>
+      </c>
+      <c r="S67"/>
+    </row>
+    <row r="68">
+      <c r="B68" t="s">
+        <v>207</v>
+      </c>
+      <c r="C68" t="s">
+        <v>208</v>
+      </c>
+      <c r="D68" t="n" s="79">
+        <v>10535.0</v>
+      </c>
+      <c r="F68" t="s">
+        <v>134</v>
+      </c>
+      <c r="G68" t="s">
+        <v>156</v>
+      </c>
+      <c r="H68" t="s">
+        <v>209</v>
+      </c>
+      <c r="I68" t="s">
+        <v>158</v>
+      </c>
+      <c r="J68" t="s">
+        <v>159</v>
+      </c>
+      <c r="K68" t="s">
+        <v>160</v>
+      </c>
+      <c r="L68" t="s">
+        <v>210</v>
+      </c>
+      <c r="M68" t="s">
+        <v>211</v>
+      </c>
+      <c r="N68"/>
+      <c r="P68" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>134</v>
+      </c>
+      <c r="R68" t="s">
+        <v>166</v>
+      </c>
+      <c r="S68"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -5129,7 +5626,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:AB55"/>
+  <dimension ref="B1:AB66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Z4" sqref="Z4"/>
@@ -5863,7 +6360,128 @@
       <c r="C55" t="s">
         <v>207</v>
       </c>
-      <c r="D55" t="n" s="68">
+      <c r="D55" s="68" t="n">
+        <v>10535.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="s">
+        <v>154</v>
+      </c>
+      <c r="C56" t="s">
+        <v>153</v>
+      </c>
+      <c r="D56" s="69" t="n">
+        <v>14198.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="s">
+        <v>163</v>
+      </c>
+      <c r="C57" t="s">
+        <v>162</v>
+      </c>
+      <c r="D57" s="70" t="n">
+        <v>15962.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="s">
+        <v>168</v>
+      </c>
+      <c r="C58" t="s">
+        <v>167</v>
+      </c>
+      <c r="D58" s="71" t="n">
+        <v>13466.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="s">
+        <v>173</v>
+      </c>
+      <c r="C59" t="s">
+        <v>172</v>
+      </c>
+      <c r="D59" s="72" t="n">
+        <v>23463.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="s">
+        <v>179</v>
+      </c>
+      <c r="C60" t="s">
+        <v>178</v>
+      </c>
+      <c r="D60" s="73" t="n">
+        <v>11085.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="s">
+        <v>185</v>
+      </c>
+      <c r="C61" t="s">
+        <v>184</v>
+      </c>
+      <c r="D61" s="74" t="n">
+        <v>21738.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="s">
+        <v>190</v>
+      </c>
+      <c r="C62" t="s">
+        <v>189</v>
+      </c>
+      <c r="D62" s="75" t="n">
+        <v>9319.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="s">
+        <v>194</v>
+      </c>
+      <c r="C63" t="s">
+        <v>193</v>
+      </c>
+      <c r="D63" s="76" t="n">
+        <v>21385.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="s">
+        <v>200</v>
+      </c>
+      <c r="C64" t="s">
+        <v>199</v>
+      </c>
+      <c r="D64" s="77" t="n">
+        <v>10690.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="s">
+        <v>204</v>
+      </c>
+      <c r="C65" t="s">
+        <v>203</v>
+      </c>
+      <c r="D65" s="78" t="n">
+        <v>11579.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="s">
+        <v>208</v>
+      </c>
+      <c r="C66" t="s">
+        <v>207</v>
+      </c>
+      <c r="D66" t="n" s="79">
         <v>10535.0</v>
       </c>
     </row>
@@ -5898,7 +6516,7 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:M49"/>
+  <dimension ref="B1:M60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
@@ -6758,10 +7376,10 @@
       <c r="C49" t="s">
         <v>207</v>
       </c>
-      <c r="D49" t="n" s="68">
+      <c r="D49" s="68" t="n">
         <v>10535.0</v>
       </c>
-      <c r="E49" t="n" s="68">
+      <c r="E49" s="68" t="n">
         <v>42678.0</v>
       </c>
       <c r="F49" t="s">
@@ -6769,6 +7387,195 @@
       </c>
       <c r="G49" s="68"/>
       <c r="H49"/>
+    </row>
+    <row r="50">
+      <c r="B50" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" t="s">
+        <v>153</v>
+      </c>
+      <c r="D50" s="69" t="n">
+        <v>14198.0</v>
+      </c>
+      <c r="E50" s="69"/>
+      <c r="F50"/>
+      <c r="G50" s="69"/>
+      <c r="H50"/>
+    </row>
+    <row r="51">
+      <c r="B51" t="s">
+        <v>163</v>
+      </c>
+      <c r="C51" t="s">
+        <v>162</v>
+      </c>
+      <c r="D51" s="70" t="n">
+        <v>15962.0</v>
+      </c>
+      <c r="E51" s="70" t="n">
+        <v>42584.0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>138</v>
+      </c>
+      <c r="G51" s="70"/>
+      <c r="H51"/>
+    </row>
+    <row r="52">
+      <c r="B52" t="s">
+        <v>168</v>
+      </c>
+      <c r="C52" t="s">
+        <v>167</v>
+      </c>
+      <c r="D52" s="71" t="n">
+        <v>13466.0</v>
+      </c>
+      <c r="E52" s="71"/>
+      <c r="F52"/>
+      <c r="G52" s="71"/>
+      <c r="H52"/>
+    </row>
+    <row r="53">
+      <c r="B53" t="s">
+        <v>173</v>
+      </c>
+      <c r="C53" t="s">
+        <v>172</v>
+      </c>
+      <c r="D53" s="72" t="n">
+        <v>23463.0</v>
+      </c>
+      <c r="E53" s="72"/>
+      <c r="F53"/>
+      <c r="G53" s="72" t="n">
+        <v>42923.0</v>
+      </c>
+      <c r="H53" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="s">
+        <v>179</v>
+      </c>
+      <c r="C54" t="s">
+        <v>178</v>
+      </c>
+      <c r="D54" s="73" t="n">
+        <v>11085.0</v>
+      </c>
+      <c r="E54" s="73" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>183</v>
+      </c>
+      <c r="G54" s="73"/>
+      <c r="H54"/>
+    </row>
+    <row r="55">
+      <c r="B55" t="s">
+        <v>185</v>
+      </c>
+      <c r="C55" t="s">
+        <v>184</v>
+      </c>
+      <c r="D55" s="74" t="n">
+        <v>21738.0</v>
+      </c>
+      <c r="E55" s="74" t="n">
+        <v>42856.0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>138</v>
+      </c>
+      <c r="G55" s="74"/>
+      <c r="H55"/>
+    </row>
+    <row r="56">
+      <c r="B56" t="s">
+        <v>190</v>
+      </c>
+      <c r="C56" t="s">
+        <v>189</v>
+      </c>
+      <c r="D56" s="75" t="n">
+        <v>9319.0</v>
+      </c>
+      <c r="E56" s="75"/>
+      <c r="F56"/>
+      <c r="G56" s="75"/>
+      <c r="H56"/>
+    </row>
+    <row r="57">
+      <c r="B57" t="s">
+        <v>194</v>
+      </c>
+      <c r="C57" t="s">
+        <v>193</v>
+      </c>
+      <c r="D57" s="76" t="n">
+        <v>21385.0</v>
+      </c>
+      <c r="E57" s="76" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>198</v>
+      </c>
+      <c r="G57" s="76"/>
+      <c r="H57"/>
+    </row>
+    <row r="58">
+      <c r="B58" t="s">
+        <v>200</v>
+      </c>
+      <c r="C58" t="s">
+        <v>199</v>
+      </c>
+      <c r="D58" s="77" t="n">
+        <v>10690.0</v>
+      </c>
+      <c r="E58" s="77"/>
+      <c r="F58"/>
+      <c r="G58" s="77"/>
+      <c r="H58"/>
+    </row>
+    <row r="59">
+      <c r="B59" t="s">
+        <v>204</v>
+      </c>
+      <c r="C59" t="s">
+        <v>203</v>
+      </c>
+      <c r="D59" s="78" t="n">
+        <v>11579.0</v>
+      </c>
+      <c r="E59" s="78"/>
+      <c r="F59"/>
+      <c r="G59" s="78"/>
+      <c r="H59"/>
+    </row>
+    <row r="60">
+      <c r="B60" t="s">
+        <v>208</v>
+      </c>
+      <c r="C60" t="s">
+        <v>207</v>
+      </c>
+      <c r="D60" t="n" s="79">
+        <v>10535.0</v>
+      </c>
+      <c r="E60" t="n" s="79">
+        <v>42678.0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>212</v>
+      </c>
+      <c r="G60" s="79"/>
+      <c r="H60"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>